<commit_message>
updated latex doc to include reformatted baseball card please help I feel ike dying is a now and later that I'm injecting into my veins
</commit_message>
<xml_diff>
--- a/Gemini Facts.xlsx
+++ b/Gemini Facts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\ENAE483_A5_CAD\ENAE483_A5_CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623881CF-3121-45A8-93FE-E8CE261E46C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4BB257-BD4B-49E8-B08B-961E03BFEAD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1335" yWindow="2115" windowWidth="28800" windowHeight="15435" xr2:uid="{5E7A8CE1-E5A6-441E-BD02-7F86C88A3349}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Program Dates:</t>
   </si>
@@ -157,6 +157,33 @@
   </si>
   <si>
     <t>Retrograde Thrusters</t>
+  </si>
+  <si>
+    <t>Launch Mass</t>
+  </si>
+  <si>
+    <t>3850 kg</t>
+  </si>
+  <si>
+    <t>Crew Size</t>
+  </si>
+  <si>
+    <t>1982 kg</t>
+  </si>
+  <si>
+    <t>Retrograde Module</t>
+  </si>
+  <si>
+    <t>Re-entry Module</t>
+  </si>
+  <si>
+    <t>591 kg</t>
+  </si>
+  <si>
+    <t>Equiptment Module</t>
+  </si>
+  <si>
+    <t>1278 kg</t>
   </si>
 </sst>
 </file>
@@ -521,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E3FB53-B2B0-49CD-BA31-4AEEA6350AB5}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,6 +774,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>